<commit_message>
modified:   client/public/fichiers/ANNEXE 14 - TABLEAU DE SUIVI DES SUBVENTIONS.xlsx
</commit_message>
<xml_diff>
--- a/client/public/fichiers/ANNEXE 14 - TABLEAU DE SUIVI DES SUBVENTIONS.xlsx
+++ b/client/public/fichiers/ANNEXE 14 - TABLEAU DE SUIVI DES SUBVENTIONS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://219295cocerto-my.sharepoint.com/personal/lgombaud_cocerto_fr/Documents/SAUVEGARDE LOCAL LG/MEMOIRE DEC/MEMOIRE/ANNEXE/ANNEXE 14 - TABLEAU DE SUIVI DES SUBVENTIONS/VERSION VIDE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lgombaud\Documents\DEF MEMOIRE\ANNEXES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="533" documentId="8_{F3F7C735-D22C-451B-BF1E-3D13E0CBE879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8FB087D-B188-4E3F-B7A5-4898D8141B1C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F056EE3D-FEBC-4FA9-A924-B1D569C3E82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D0ACEEF9-5891-46BB-A4B6-D1E39F4BA593}"/>
   </bookViews>
@@ -894,7 +894,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B31"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1161,19 +1161,18 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="48" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="16" customWidth="1"/>
     <col min="2" max="2" width="46.5703125" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" style="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.140625" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" style="16" customWidth="1"/>
     <col min="6" max="7" width="15.140625" style="16" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" style="17" customWidth="1"/>
-    <col min="9" max="9" width="23" style="17" customWidth="1"/>
+    <col min="8" max="9" width="18.7109375" style="17" customWidth="1"/>
     <col min="10" max="10" width="20.5703125" style="16" customWidth="1"/>
     <col min="11" max="11" width="19.140625" style="17" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" style="17" customWidth="1"/>
@@ -29863,7 +29862,7 @@
       <c r="V868" s="11"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:V1"/>
   </mergeCells>

</xml_diff>